<commit_message>
Added changes for cart in FE00
5.	Recoded Cartridge bank switching to only exist when MiSTer slot 3 is selected. [removed soft multipak select]
13. Fixed incorrect addressing of FE00-FEFF for CARTs which gets PITFALL and RAMPAGE working
</commit_message>
<xml_diff>
--- a/COCO3_Comp.xlsx
+++ b/COCO3_Comp.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stan.HODGEHOUSE\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\MISTer\CoCo3_Mister\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9C748E-54B1-424B-BC22-B54DD96BD9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5010A38A-A721-4648-B47A-A8C3BB40B2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16416" yWindow="1368" windowWidth="23856" windowHeight="13092" xr2:uid="{57A7BCA7-2C65-4EF6-A914-7E4BBD33BE36}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="44">
   <si>
     <t>Cart</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Branch 0001</t>
+  </si>
+  <si>
+    <t>Popstar Demo</t>
   </si>
 </sst>
 </file>
@@ -542,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B1C0CF-A4E7-4A2B-AD36-22ADB22CD812}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1019,27 +1022,38 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B34" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="35" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="36" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix PIA2 adrs, added Auto Run
1.	Changed PIA 2 addressing to align with real CoCo3 hardware and end at FF2F.
2.	Removal of 16 bit sound extentions as they overlap speach / sound cart.  This is
	accompanied by a rework of the sound mixing to be more correct.
3.	Re-arranged MiSTer drive LUNs to support future auto-boot from SDC drive 0
4.	Added 'Auto Run' feature.  You must use slot 2 [SDC].  Take your floopy or HD
	and copy it to a file name of 'boot.vhd'.  This will be auto mounted to drive 0
	on the SDC.  In the menu, find a new item Auto Run:.  It can be set to No, DOS or
	AUTO.BAS.  Choosing dos causes the 'DOS' command to be executed on power up.  Setting
	the option to 'AUTO.BAS' will cause a 'RUN"AUTO' command to be executed upon powerup.
	Save your settings to cause the changes to be remembered.  The Auto Run system re-arms
	upon using the 'Cold Boot' menu item.

To Do...
1.	Add Speech / Music cart
2.	Fix Color File II
3.	Fic Castle of Tharoggad
</commit_message>
<xml_diff>
--- a/COCO3_Comp.xlsx
+++ b/COCO3_Comp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\MISTer\CoCo3_Mister\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F8F7D7-1CF0-42A5-B736-9ECFBE435FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA23B68B-2ADD-44FC-8659-8DC75A2D5A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15996" yWindow="2760" windowWidth="23856" windowHeight="13092" xr2:uid="{57A7BCA7-2C65-4EF6-A914-7E4BBD33BE36}"/>
+    <workbookView xWindow="13632" yWindow="3240" windowWidth="23856" windowHeight="13092" xr2:uid="{57A7BCA7-2C65-4EF6-A914-7E4BBD33BE36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="45">
   <si>
     <t>Cart</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>Load 20240205</t>
+  </si>
+  <si>
+    <t>Load 20240216</t>
   </si>
 </sst>
 </file>
@@ -530,14 +533,13 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="11.109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -551,7 +553,9 @@
       <c r="C1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -566,7 +570,9 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -578,7 +584,9 @@
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -590,7 +598,9 @@
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -602,7 +612,9 @@
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -614,7 +626,9 @@
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -626,7 +640,9 @@
       <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -638,7 +654,9 @@
       <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -650,7 +668,9 @@
       <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -662,7 +682,9 @@
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -674,7 +696,9 @@
       <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -686,7 +710,9 @@
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -698,7 +724,9 @@
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -710,7 +738,9 @@
       <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -722,7 +752,9 @@
       <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -734,7 +766,9 @@
       <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -746,7 +780,9 @@
       <c r="C17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -758,7 +794,9 @@
       <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -770,7 +808,9 @@
       <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -782,7 +822,9 @@
       <c r="C20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -794,7 +836,9 @@
       <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -806,7 +850,9 @@
       <c r="C22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -818,7 +864,9 @@
       <c r="C23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -830,7 +878,9 @@
       <c r="C24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -842,7 +892,9 @@
       <c r="C26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -854,7 +906,9 @@
       <c r="C27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -866,7 +920,9 @@
       <c r="C28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -878,7 +934,9 @@
       <c r="C29" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -890,7 +948,9 @@
       <c r="C30" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="2"/>
+      <c r="D30" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -902,9 +962,11 @@
       <c r="C31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="34" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D31" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -914,8 +976,11 @@
       <c r="C34" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D34" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -925,8 +990,11 @@
       <c r="C35" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D35" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -936,8 +1004,11 @@
       <c r="C36" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D36" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -947,8 +1018,11 @@
       <c r="C37" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D37" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -956,6 +1030,9 @@
         <v>42</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>